<commit_message>
Add a retry flowchart loop and a cRetryLimit config variable
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -19,12 +19,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Description</t>
   </si>
   <si>
     <t>Entries</t>
+  </si>
+  <si>
+    <t>RetryLimit</t>
   </si>
 </sst>
 </file>
@@ -342,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -358,20 +361,26 @@
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
       <c r="B2">
         <v>1</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add the destination email in the config and the source email and password as a windows credentials name
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Description</t>
   </si>
@@ -28,16 +28,36 @@
   </si>
   <si>
     <t>RetryLimit</t>
+  </si>
+  <si>
+    <t>burcea.bogdan.madalin@gmail.com</t>
+  </si>
+  <si>
+    <t>DestinationEmail</t>
+  </si>
+  <si>
+    <t>SourceEmailCredential</t>
+  </si>
+  <si>
+    <t>bot_gmail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,13 +80,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -345,10 +368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -356,12 +379,12 @@
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="32" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -371,8 +394,14 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
@@ -382,9 +411,21 @@
       <c r="C2">
         <v>3</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add a ScrapeAmount config variable and modify readme
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Description</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>bot_gmail</t>
+  </si>
+  <si>
+    <t>ScrapeAmount</t>
   </si>
 </sst>
 </file>
@@ -368,23 +371,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="32" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" customWidth="1"/>
-    <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -392,38 +395,44 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>5</v>
+      <c r="F1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>400</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="F2">
+        <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>